<commit_message>
finished seeding starting stocktransaction
</commit_message>
<xml_diff>
--- a/Project_SLAY/Copy of Longhorn Bank Data 2022 v1.xlsx
+++ b/Project_SLAY/Copy of Longhorn Bank Data 2022 v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steven/Desktop/MIS333K/Project_S.L.A.Y/Project_SLAY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738F94A8-D5D9-4040-897B-1A2033A828B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F78A48-EAEE-C546-B65C-F53D238D5D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19160" yWindow="500" windowWidth="14440" windowHeight="18840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5900" yWindow="500" windowWidth="27700" windowHeight="18840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="485">
   <si>
     <t>EmailAddress</t>
   </si>
@@ -1498,6 +1498,9 @@
   <si>
     <t>Year</t>
   </si>
+  <si>
+    <t>transfer</t>
+  </si>
 </sst>
 </file>
 
@@ -1508,7 +1511,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1583,6 +1586,21 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1610,7 +1628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1684,6 +1702,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16474,7 +16494,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -20951,7 +20971,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -20977,7 +20997,7 @@
       <c r="C1" s="29" t="s">
         <v>456</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="43" t="s">
         <v>457</v>
       </c>
       <c r="E1" s="29" t="s">
@@ -20997,8 +21017,8 @@
       <c r="A2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>460</v>
+      <c r="B2" s="44" t="s">
+        <v>484</v>
       </c>
       <c r="D2" s="6">
         <v>2290000021</v>
@@ -21020,8 +21040,8 @@
       <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>460</v>
+      <c r="B3" s="44" t="s">
+        <v>484</v>
       </c>
       <c r="D3" s="6">
         <v>2290000024</v>

</xml_diff>